<commit_message>
Punto de partida, Se agrego escenarios de diferentes precios
</commit_message>
<xml_diff>
--- a/DataBases/Prices_Fuels/HighPrice_Oil_AEO_2019/Price_AEO_HighOil.xlsx
+++ b/DataBases/Prices_Fuels/HighPrice_Oil_AEO_2019/Price_AEO_HighOil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\DataBases\Prices_Fuels\HighPrice_Oil_AEO_2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95F7751-E1AD-4F5A-80BD-2ED209AAB747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B128DF-9AB9-4962-AB18-C776A0045B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ditillate Fuel Oil" sheetId="2" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="150">
   <si>
     <t>USD2019/MillonBTU</t>
   </si>
@@ -537,6 +537,9 @@
   </si>
   <si>
     <t>MBTU/gal</t>
+  </si>
+  <si>
+    <t>AVGAS</t>
   </si>
 </sst>
 </file>
@@ -1681,7 +1684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:W65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:M38"/>
     </sheetView>
   </sheetViews>
@@ -3728,8 +3731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF74EBC4-D036-481C-A956-1BCD48200948}">
   <dimension ref="D4:S45"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S38" sqref="P38:S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3746,8 +3749,8 @@
     <col min="14" max="14" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="4:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="4:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="4:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D5" s="17" t="s">
         <v>0</v>
       </c>
@@ -3762,7 +3765,7 @@
       <c r="M5" s="18"/>
       <c r="N5" s="19"/>
     </row>
-    <row r="6" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
@@ -3802,8 +3805,11 @@
       <c r="Q6" s="12" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="7" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D7" s="5">
         <v>2019</v>
       </c>
@@ -3839,10 +3845,13 @@
       </c>
       <c r="P7">
         <f>+P8*(100%-Q8)</f>
-        <v>1.8960538207374225</v>
-      </c>
-    </row>
-    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
+        <v>15.775408175707556</v>
+      </c>
+      <c r="S7">
+        <v>15.775408175707556</v>
+      </c>
+    </row>
+    <row r="8" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D8" s="4">
         <v>2020</v>
       </c>
@@ -3877,15 +3886,18 @@
         <v>34.096516000000001</v>
       </c>
       <c r="P8" s="14">
-        <f>+R42</f>
-        <v>2.6850000000000001</v>
+        <f>+R43</f>
+        <v>22.339540412044375</v>
       </c>
       <c r="Q8" s="13">
         <f>+(F8-$F$7)/$F$7</f>
         <v>0.29383470363596931</v>
       </c>
-    </row>
-    <row r="9" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S8">
+        <v>22.339540412044375</v>
+      </c>
+    </row>
+    <row r="9" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D9" s="5">
         <v>2021</v>
       </c>
@@ -3921,14 +3933,17 @@
       </c>
       <c r="P9">
         <f>+$P$8*(100%+Q9)</f>
-        <v>3.6721515655846493</v>
+        <v>30.552766591631393</v>
       </c>
       <c r="Q9" s="13">
-        <f t="shared" ref="Q9:Q38" si="0">+(F9-$F$7)/$F$7</f>
+        <f t="shared" ref="Q9:Q37" si="0">+(F9-$F$7)/$F$7</f>
         <v>0.36765421437044665</v>
       </c>
-    </row>
-    <row r="10" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S9">
+        <v>30.552766591631393</v>
+      </c>
+    </row>
+    <row r="10" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D10" s="4">
         <v>2022</v>
       </c>
@@ -3964,14 +3979,17 @@
       </c>
       <c r="P10">
         <f t="shared" ref="P10:P38" si="1">+$P$8*(100%+Q10)</f>
-        <v>3.9488455843461479</v>
+        <v>32.85489590779283</v>
       </c>
       <c r="Q10" s="13">
         <f t="shared" si="0"/>
         <v>0.47070599044549272</v>
       </c>
-    </row>
-    <row r="11" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S10">
+        <v>32.85489590779283</v>
+      </c>
+    </row>
+    <row r="11" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D11" s="5">
         <v>2023</v>
       </c>
@@ -4007,14 +4025,17 @@
       </c>
       <c r="P11">
         <f t="shared" si="1"/>
-        <v>4.3658679419669966</v>
+        <v>36.324574794495611</v>
       </c>
       <c r="Q11" s="13">
         <f t="shared" si="0"/>
         <v>0.62602157987597618</v>
       </c>
-    </row>
-    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S11">
+        <v>36.324574794495611</v>
+      </c>
+    </row>
+    <row r="12" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D12" s="4">
         <v>2024</v>
       </c>
@@ -4050,14 +4071,17 @@
       </c>
       <c r="P12">
         <f t="shared" si="1"/>
-        <v>4.5756499114680862</v>
+        <v>38.06998737750785</v>
       </c>
       <c r="Q12" s="13">
         <f t="shared" si="0"/>
         <v>0.70415266721343994</v>
       </c>
-    </row>
-    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S12">
+        <v>38.06998737750785</v>
+      </c>
+    </row>
+    <row r="13" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D13" s="5">
         <v>2025</v>
       </c>
@@ -4093,14 +4117,17 @@
       </c>
       <c r="P13">
         <f t="shared" si="1"/>
-        <v>4.7155582906360261</v>
+        <v>39.23404283017296</v>
       </c>
       <c r="Q13" s="13">
         <f t="shared" si="0"/>
         <v>0.75626007100038206</v>
       </c>
-    </row>
-    <row r="14" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S13">
+        <v>39.23404283017296</v>
+      </c>
+    </row>
+    <row r="14" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D14" s="4">
         <v>2026</v>
       </c>
@@ -4136,14 +4163,17 @@
       </c>
       <c r="P14">
         <f t="shared" si="1"/>
-        <v>4.8286006196414357</v>
+        <v>40.174569339330489</v>
       </c>
       <c r="Q14" s="13">
         <f t="shared" si="0"/>
         <v>0.79836149707316029</v>
       </c>
-    </row>
-    <row r="15" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S14">
+        <v>40.174569339330489</v>
+      </c>
+    </row>
+    <row r="15" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D15" s="5">
         <v>2027</v>
       </c>
@@ -4179,14 +4209,17 @@
       </c>
       <c r="P15">
         <f t="shared" si="1"/>
-        <v>4.8298770036817036</v>
+        <v>40.185189016369165</v>
       </c>
       <c r="Q15" s="13">
         <f t="shared" si="0"/>
         <v>0.7988368728795916</v>
       </c>
-    </row>
-    <row r="16" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S15">
+        <v>40.185189016369165</v>
+      </c>
+    </row>
+    <row r="16" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D16" s="4">
         <v>2028</v>
       </c>
@@ -4222,14 +4255,17 @@
       </c>
       <c r="P16">
         <f t="shared" si="1"/>
-        <v>4.9155231063377434</v>
+        <v>40.897775448927341</v>
       </c>
       <c r="Q16" s="13">
         <f>+(F16-$F$7)/$F$7</f>
         <v>0.83073486269562125</v>
       </c>
-    </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S16">
+        <v>40.897775448927341</v>
+      </c>
+    </row>
+    <row r="17" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D17" s="5">
         <v>2029</v>
       </c>
@@ -4265,14 +4301,17 @@
       </c>
       <c r="P17">
         <f t="shared" si="1"/>
-        <v>5.186026845892453</v>
+        <v>43.14840085726685</v>
       </c>
       <c r="Q17" s="13">
         <f t="shared" si="0"/>
         <v>0.93148113441059699</v>
       </c>
-    </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S17">
+        <v>43.14840085726685</v>
+      </c>
+    </row>
+    <row r="18" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D18" s="4">
         <v>2030</v>
       </c>
@@ -4308,14 +4347,17 @@
       </c>
       <c r="P18">
         <f t="shared" si="1"/>
-        <v>5.228201802220716</v>
+        <v>43.4993018409806</v>
       </c>
       <c r="Q18" s="13">
         <f t="shared" si="0"/>
         <v>0.94718875315482876</v>
       </c>
-    </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S18">
+        <v>43.4993018409806</v>
+      </c>
+    </row>
+    <row r="19" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D19" s="5">
         <v>2031</v>
       </c>
@@ -4351,14 +4393,17 @@
       </c>
       <c r="P19">
         <f t="shared" si="1"/>
-        <v>5.3469594341880446</v>
+        <v>44.487380395383894</v>
       </c>
       <c r="Q19" s="13">
         <f t="shared" si="0"/>
         <v>0.9914187836826982</v>
       </c>
-    </row>
-    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S19">
+        <v>44.487380395383894</v>
+      </c>
+    </row>
+    <row r="20" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D20" s="4">
         <v>2032</v>
       </c>
@@ -4394,14 +4439,17 @@
       </c>
       <c r="P20">
         <f t="shared" si="1"/>
-        <v>5.5531262659612883</v>
+        <v>46.202714574162862</v>
       </c>
       <c r="Q20" s="13">
         <f t="shared" si="0"/>
         <v>1.0682034510097911</v>
       </c>
-    </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S20">
+        <v>46.202714574162862</v>
+      </c>
+    </row>
+    <row r="21" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D21" s="5">
         <v>2033</v>
       </c>
@@ -4437,14 +4485,17 @@
       </c>
       <c r="P21">
         <f t="shared" si="1"/>
-        <v>5.594502565321827</v>
+        <v>46.546970630649113</v>
       </c>
       <c r="Q21" s="13">
         <f t="shared" si="0"/>
         <v>1.0836136183693954</v>
       </c>
-    </row>
-    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S21">
+        <v>46.546970630649113</v>
+      </c>
+    </row>
+    <row r="22" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D22" s="4">
         <v>2034</v>
       </c>
@@ -4480,14 +4531,17 @@
       </c>
       <c r="P22">
         <f t="shared" si="1"/>
-        <v>5.6356855731912097</v>
+        <v>46.8896184774229</v>
       </c>
       <c r="Q22" s="13">
         <f t="shared" si="0"/>
         <v>1.0989517963468192</v>
       </c>
-    </row>
-    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S22">
+        <v>46.8896184774229</v>
+      </c>
+    </row>
+    <row r="23" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D23" s="5">
         <v>2035</v>
       </c>
@@ -4523,14 +4577,17 @@
       </c>
       <c r="P23">
         <f t="shared" si="1"/>
-        <v>5.6957885904069165</v>
+        <v>47.389683200691465</v>
       </c>
       <c r="Q23" s="13">
         <f t="shared" si="0"/>
         <v>1.121336532740006</v>
       </c>
-    </row>
-    <row r="24" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S23">
+        <v>47.389683200691465</v>
+      </c>
+    </row>
+    <row r="24" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D24" s="4">
         <v>2036</v>
       </c>
@@ -4566,14 +4623,17 @@
       </c>
       <c r="P24">
         <f t="shared" si="1"/>
-        <v>5.790142896533089</v>
+        <v>48.174722990172299</v>
       </c>
       <c r="Q24" s="13">
         <f t="shared" si="0"/>
         <v>1.1564778013158619</v>
       </c>
-    </row>
-    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S24">
+        <v>48.174722990172299</v>
+      </c>
+    </row>
+    <row r="25" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D25" s="5">
         <v>2037</v>
       </c>
@@ -4609,14 +4669,17 @@
       </c>
       <c r="P25">
         <f t="shared" si="1"/>
-        <v>5.8491884955912985</v>
+        <v>48.665989860307953</v>
       </c>
       <c r="Q25" s="13">
         <f t="shared" si="0"/>
         <v>1.1784687134418246</v>
       </c>
-    </row>
-    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S25">
+        <v>48.665989860307953</v>
+      </c>
+    </row>
+    <row r="26" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D26" s="4">
         <v>2038</v>
       </c>
@@ -4652,14 +4715,17 @@
       </c>
       <c r="P26">
         <f t="shared" si="1"/>
-        <v>5.9081099406272006</v>
+        <v>49.156223753237413</v>
       </c>
       <c r="Q26" s="13">
         <f t="shared" si="0"/>
         <v>1.2004133857084549</v>
       </c>
-    </row>
-    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S26">
+        <v>49.156223753237413</v>
+      </c>
+    </row>
+    <row r="27" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D27" s="5">
         <v>2039</v>
       </c>
@@ -4695,14 +4761,17 @@
       </c>
       <c r="P27">
         <f t="shared" si="1"/>
-        <v>5.9552450060268924</v>
+        <v>49.548393473282388</v>
       </c>
       <c r="Q27" s="13">
         <f t="shared" si="0"/>
         <v>1.2179683448889729</v>
       </c>
-    </row>
-    <row r="28" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S27">
+        <v>49.548393473282388</v>
+      </c>
+    </row>
+    <row r="28" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D28" s="4">
         <v>2040</v>
       </c>
@@ -4738,14 +4807,17 @@
       </c>
       <c r="P28">
         <f t="shared" si="1"/>
-        <v>6.0486370726330527</v>
+        <v>50.325427307961213</v>
       </c>
       <c r="Q28" s="13">
         <f t="shared" si="0"/>
         <v>1.2527512374797216</v>
       </c>
-    </row>
-    <row r="29" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S28">
+        <v>50.325427307961213</v>
+      </c>
+    </row>
+    <row r="29" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D29" s="5">
         <v>2041</v>
       </c>
@@ -4781,14 +4853,17 @@
       </c>
       <c r="P29">
         <f t="shared" si="1"/>
-        <v>6.1060761883302348</v>
+        <v>50.803328032858531</v>
       </c>
       <c r="Q29" s="13">
         <f t="shared" si="0"/>
         <v>1.274143831780348</v>
       </c>
-    </row>
-    <row r="30" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S29">
+        <v>50.803328032858531</v>
+      </c>
+    </row>
+    <row r="30" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D30" s="4">
         <v>2042</v>
       </c>
@@ -4824,14 +4899,17 @@
       </c>
       <c r="P30">
         <f t="shared" si="1"/>
-        <v>6.1526299121483659</v>
+        <v>51.190660917240763</v>
       </c>
       <c r="Q30" s="13">
         <f t="shared" si="0"/>
         <v>1.2914822764053506</v>
       </c>
-    </row>
-    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S30">
+        <v>51.190660917240763</v>
+      </c>
+    </row>
+    <row r="31" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D31" s="5">
         <v>2043</v>
       </c>
@@ -4867,14 +4945,17 @@
       </c>
       <c r="P31">
         <f t="shared" si="1"/>
-        <v>6.2133148211111671</v>
+        <v>51.695567053619065</v>
       </c>
       <c r="Q31" s="13">
         <f t="shared" si="0"/>
         <v>1.3140837322574179</v>
       </c>
-    </row>
-    <row r="32" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="S31">
+        <v>51.695567053619065</v>
+      </c>
+    </row>
+    <row r="32" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D32" s="4">
         <v>2044</v>
       </c>
@@ -4910,12 +4991,15 @@
       </c>
       <c r="P32">
         <f t="shared" si="1"/>
-        <v>6.2727350828984374</v>
+        <v>52.189951165161332</v>
       </c>
       <c r="Q32" s="13">
         <f t="shared" si="0"/>
         <v>1.3362141835748373</v>
       </c>
+      <c r="S32">
+        <v>52.189951165161332</v>
+      </c>
     </row>
     <row r="33" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D33" s="5">
@@ -4953,12 +5037,15 @@
       </c>
       <c r="P33">
         <f t="shared" si="1"/>
-        <v>6.3247614866777297</v>
+        <v>52.622817440662566</v>
       </c>
       <c r="Q33" s="13">
         <f t="shared" si="0"/>
         <v>1.3555908702710353</v>
       </c>
+      <c r="S33">
+        <v>52.622817440662566</v>
+      </c>
     </row>
     <row r="34" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D34" s="4">
@@ -4996,12 +5083,15 @@
       </c>
       <c r="P34">
         <f t="shared" si="1"/>
-        <v>6.3751131865697044</v>
+        <v>53.041749967497545</v>
       </c>
       <c r="Q34" s="13">
         <f t="shared" si="0"/>
         <v>1.3743438311246572</v>
       </c>
+      <c r="S34">
+        <v>53.041749967497545</v>
+      </c>
     </row>
     <row r="35" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D35" s="5">
@@ -5039,12 +5129,15 @@
       </c>
       <c r="P35">
         <f t="shared" si="1"/>
-        <v>6.4009672989255968</v>
+        <v>53.2568594601575</v>
       </c>
       <c r="Q35" s="13">
         <f t="shared" si="0"/>
         <v>1.3839729232497564</v>
       </c>
+      <c r="S35">
+        <v>53.2568594601575</v>
+      </c>
     </row>
     <row r="36" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D36" s="4">
@@ -5082,12 +5175,15 @@
       </c>
       <c r="P36">
         <f t="shared" si="1"/>
-        <v>6.4332546802660575</v>
+        <v>53.525494566397469</v>
       </c>
       <c r="Q36" s="13">
         <f t="shared" si="0"/>
         <v>1.3959980187210645</v>
       </c>
+      <c r="S36">
+        <v>53.525494566397469</v>
+      </c>
     </row>
     <row r="37" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D37" s="5">
@@ -5125,12 +5221,15 @@
       </c>
       <c r="P37">
         <f t="shared" si="1"/>
-        <v>6.4768980284061648</v>
+        <v>53.888612756152725</v>
       </c>
       <c r="Q37" s="13">
         <f t="shared" si="0"/>
         <v>1.4122525245460575</v>
       </c>
+      <c r="S37">
+        <v>53.888612756152725</v>
+      </c>
     </row>
     <row r="38" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D38" s="4">
@@ -5168,11 +5267,14 @@
       </c>
       <c r="P38">
         <f t="shared" si="1"/>
-        <v>6.501639889439609</v>
+        <v>54.09446817679548</v>
       </c>
       <c r="Q38" s="13">
-        <f t="shared" si="0"/>
+        <f>+(F38-$F$7)/$F$7</f>
         <v>1.4214673703685696</v>
+      </c>
+      <c r="S38">
+        <v>54.09446817679548</v>
       </c>
     </row>
     <row r="42" spans="4:19" x14ac:dyDescent="0.25">

</xml_diff>